<commit_message>
Uj enkoderen is mukodik a SW, ki kellet venni a QCNT presqualer-t es igy mar jo
</commit_message>
<xml_diff>
--- a/Meresi_adatok/Szog_ugras_megoldas.xlsx
+++ b/Meresi_adatok/Szog_ugras_megoldas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ti\Workspace\SIN_COS_FROM_EMPTY\Meresi_adatok\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A6F5680-A0D8-4E0D-AE40-FEE4A5808657}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{917093FE-ACFE-46D2-B6D2-77C48CFCDCBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{49F48117-8158-4304-A18F-900A4818AF77}"/>
   </bookViews>
@@ -176,10 +176,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2582,2407 +2582,6 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="hu-HU"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="hu-HU"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="smoothMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Munka1!$K$4:$K$203</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="200"/>
-                <c:pt idx="0">
-                  <c:v>158.86680472900591</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>174.14277388246717</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>192.52356420413156</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>208.56171007803857</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>221.6667585569424</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>232.109719118051</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>242.43129990063855</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>258.90156105354959</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>277.91750303482831</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>299.36082027615629</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>321.33168205051533</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>342.37056266550377</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.83315620018080949</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>16.075038107193635</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>29.378728201834704</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>39.009772360349437</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>50.615501756264813</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>65.268650658673209</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>82.375807495548173</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>101.40447987914702</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>115.86757179461415</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>125.80166671687783</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>133.1992045906602</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>140.07450889640305</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>147.83854648892412</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>158.80255253337523</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>175.00349805033593</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>192.24010031543077</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>208.54717411885235</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>221.68131337037516</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>231.22358371204078</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>243.17258886245082</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>258.80538930150874</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>276.84711400197966</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>299.50515140086139</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>321.07079146141695</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>342.5204610219663</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>0.63713809360231721</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>16.859711897238952</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>29.262256783380494</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>39.03818989633934</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>50.615501756264813</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>64.485146645778826</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>82.611232327209009</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>101.06508020597587</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>115.06025419596952</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>125.59649294275776</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>133.02306257013521</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>139.83123590502177</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>147.4704617216689</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>158.77512184750483</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>174.97016389785909</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>192.37613163884646</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>209.52136183458163</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>221.37298900645314</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>231.62830983179663</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>243.25695077090867</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>257.13724898104181</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>277.1446583705914</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>298.7303530077404</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>320.87623300778654</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>341.56505117707798</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>1.443289437959109</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>17.253462914086839</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>28.880125031434297</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>39.271244633761768</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>50.02755405510559</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>64.232168466203632</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>83.176959256210424</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>99.581704823521662</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>115.17961891252526</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>125.49856137578639</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>132.7996267442409</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>139.59012089015792</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>147.46432177181862</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>158.70547251071892</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>174.30367255550289</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>192.76373214008527</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>208.16833124175849</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>221.32264923361345</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>231.9221603847088</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>242.57925749105476</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>257.80837496853343</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>276.54799337985577</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>297.67865178651107</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>319.91413917850628</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>341.19691747275118</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>0.54565759341571152</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>16.063275519197077</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>29.012757933925535</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>38.335658243374823</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>49.853696003748446</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>65.018260896983307</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>81.333515281591389</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>100.39601948946836</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>114.84770277489227</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>125.06490230654919</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>132.6237045662468</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>139.27907162220669</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>147.01639405282813</c:v>
-                </c:pt>
-                <c:pt idx="100">
-                  <c:v>158.00807467267046</c:v>
-                </c:pt>
-                <c:pt idx="101">
-                  <c:v>173.82854188596994</c:v>
-                </c:pt>
-                <c:pt idx="102">
-                  <c:v>190.90940259046528</c:v>
-                </c:pt>
-                <c:pt idx="103">
-                  <c:v>207.67359348972192</c:v>
-                </c:pt>
-                <c:pt idx="104">
-                  <c:v>220.94105516138956</c:v>
-                </c:pt>
-                <c:pt idx="105">
-                  <c:v>231.26572013776575</c:v>
-                </c:pt>
-                <c:pt idx="106">
-                  <c:v>242.5822189474751</c:v>
-                </c:pt>
-                <c:pt idx="107">
-                  <c:v>257.16379767802675</c:v>
-                </c:pt>
-                <c:pt idx="108">
-                  <c:v>274.92620116880931</c:v>
-                </c:pt>
-                <c:pt idx="109">
-                  <c:v>297.34987578006985</c:v>
-                </c:pt>
-                <c:pt idx="110">
-                  <c:v>318.83959633795348</c:v>
-                </c:pt>
-                <c:pt idx="111">
-                  <c:v>339.52441763490663</c:v>
-                </c:pt>
-                <c:pt idx="112">
-                  <c:v>358.47836198416087</c:v>
-                </c:pt>
-                <c:pt idx="113">
-                  <c:v>15.127564653005578</c:v>
-                </c:pt>
-                <c:pt idx="114">
-                  <c:v>26.963063752595701</c:v>
-                </c:pt>
-                <c:pt idx="115">
-                  <c:v>37.978928193429823</c:v>
-                </c:pt>
-                <c:pt idx="116">
-                  <c:v>49.705617997190238</c:v>
-                </c:pt>
-                <c:pt idx="117">
-                  <c:v>63.072995907817315</c:v>
-                </c:pt>
-                <c:pt idx="118">
-                  <c:v>81.36349097952727</c:v>
-                </c:pt>
-                <c:pt idx="119">
-                  <c:v>99.149933943058727</c:v>
-                </c:pt>
-                <c:pt idx="120">
-                  <c:v>114.07725482444224</c:v>
-                </c:pt>
-                <c:pt idx="121">
-                  <c:v>124.76519723657678</c:v>
-                </c:pt>
-                <c:pt idx="122">
-                  <c:v>131.90436640955625</c:v>
-                </c:pt>
-                <c:pt idx="123">
-                  <c:v>138.77164780908345</c:v>
-                </c:pt>
-                <c:pt idx="124">
-                  <c:v>146.15875662559532</c:v>
-                </c:pt>
-                <c:pt idx="125">
-                  <c:v>157.094810135144</c:v>
-                </c:pt>
-                <c:pt idx="126">
-                  <c:v>171.33002406433889</c:v>
-                </c:pt>
-                <c:pt idx="127">
-                  <c:v>189.95146953323484</c:v>
-                </c:pt>
-                <c:pt idx="128">
-                  <c:v>206.75414547242175</c:v>
-                </c:pt>
-                <c:pt idx="129">
-                  <c:v>219.39693911113142</c:v>
-                </c:pt>
-                <c:pt idx="130">
-                  <c:v>230.6742264146695</c:v>
-                </c:pt>
-                <c:pt idx="131">
-                  <c:v>241.23006093652356</c:v>
-                </c:pt>
-                <c:pt idx="132">
-                  <c:v>255.15847063591119</c:v>
-                </c:pt>
-                <c:pt idx="133">
-                  <c:v>274.58007041519295</c:v>
-                </c:pt>
-                <c:pt idx="134">
-                  <c:v>295.5260598398761</c:v>
-                </c:pt>
-                <c:pt idx="135">
-                  <c:v>316.92453729174849</c:v>
-                </c:pt>
-                <c:pt idx="136">
-                  <c:v>337.8768718046548</c:v>
-                </c:pt>
-                <c:pt idx="137">
-                  <c:v>357.46731891187983</c:v>
-                </c:pt>
-                <c:pt idx="138">
-                  <c:v>12.974318335215045</c:v>
-                </c:pt>
-                <c:pt idx="139">
-                  <c:v>26.167564534558977</c:v>
-                </c:pt>
-                <c:pt idx="140">
-                  <c:v>37.555686992892497</c:v>
-                </c:pt>
-                <c:pt idx="141">
-                  <c:v>47.243301383155952</c:v>
-                </c:pt>
-                <c:pt idx="142">
-                  <c:v>61.724819850870134</c:v>
-                </c:pt>
-                <c:pt idx="143">
-                  <c:v>79.602220008826464</c:v>
-                </c:pt>
-                <c:pt idx="144">
-                  <c:v>96.854329640693891</c:v>
-                </c:pt>
-                <c:pt idx="145">
-                  <c:v>113.30552983692257</c:v>
-                </c:pt>
-                <c:pt idx="146">
-                  <c:v>124.03076016957527</c:v>
-                </c:pt>
-                <c:pt idx="147">
-                  <c:v>131.45266696615792</c:v>
-                </c:pt>
-                <c:pt idx="148">
-                  <c:v>138.24078988019465</c:v>
-                </c:pt>
-                <c:pt idx="149">
-                  <c:v>145.72094198334636</c:v>
-                </c:pt>
-                <c:pt idx="150">
-                  <c:v>155.70975095328043</c:v>
-                </c:pt>
-                <c:pt idx="151">
-                  <c:v>170.17264251996562</c:v>
-                </c:pt>
-                <c:pt idx="152">
-                  <c:v>188.66826942714931</c:v>
-                </c:pt>
-                <c:pt idx="153">
-                  <c:v>205.10276838309102</c:v>
-                </c:pt>
-                <c:pt idx="154">
-                  <c:v>218.56858418742968</c:v>
-                </c:pt>
-                <c:pt idx="155">
-                  <c:v>229.76871301125755</c:v>
-                </c:pt>
-                <c:pt idx="156">
-                  <c:v>239.50962533089705</c:v>
-                </c:pt>
-                <c:pt idx="157">
-                  <c:v>254.78622023602668</c:v>
-                </c:pt>
-                <c:pt idx="158">
-                  <c:v>272.7214281083281</c:v>
-                </c:pt>
-                <c:pt idx="159">
-                  <c:v>293.18410725321019</c:v>
-                </c:pt>
-                <c:pt idx="160">
-                  <c:v>315.2291818957541</c:v>
-                </c:pt>
-                <c:pt idx="161">
-                  <c:v>336.46528557205369</c:v>
-                </c:pt>
-                <c:pt idx="162">
-                  <c:v>355.76176520031515</c:v>
-                </c:pt>
-                <c:pt idx="163">
-                  <c:v>11.540962590915683</c:v>
-                </c:pt>
-                <c:pt idx="164">
-                  <c:v>26.276167341797368</c:v>
-                </c:pt>
-                <c:pt idx="165">
-                  <c:v>36.036655059979985</c:v>
-                </c:pt>
-                <c:pt idx="166">
-                  <c:v>46.737583940110618</c:v>
-                </c:pt>
-                <c:pt idx="167">
-                  <c:v>60.424373340184296</c:v>
-                </c:pt>
-                <c:pt idx="168">
-                  <c:v>76.880315577792572</c:v>
-                </c:pt>
-                <c:pt idx="169">
-                  <c:v>96.512866392125517</c:v>
-                </c:pt>
-                <c:pt idx="170">
-                  <c:v>111.96124166766432</c:v>
-                </c:pt>
-                <c:pt idx="171">
-                  <c:v>123.11442702280245</c:v>
-                </c:pt>
-                <c:pt idx="172">
-                  <c:v>130.95958211875612</c:v>
-                </c:pt>
-                <c:pt idx="173">
-                  <c:v>137.8595504289286</c:v>
-                </c:pt>
-                <c:pt idx="174">
-                  <c:v>145.01137390009936</c:v>
-                </c:pt>
-                <c:pt idx="175">
-                  <c:v>154.54602403565306</c:v>
-                </c:pt>
-                <c:pt idx="176">
-                  <c:v>169.319462726328</c:v>
-                </c:pt>
-                <c:pt idx="177">
-                  <c:v>186.11377000967605</c:v>
-                </c:pt>
-                <c:pt idx="178">
-                  <c:v>203.55001695579466</c:v>
-                </c:pt>
-                <c:pt idx="179">
-                  <c:v>218.1445342435261</c:v>
-                </c:pt>
-                <c:pt idx="180">
-                  <c:v>228.12099779868771</c:v>
-                </c:pt>
-                <c:pt idx="181">
-                  <c:v>239.35354280060201</c:v>
-                </c:pt>
-                <c:pt idx="182">
-                  <c:v>252.7960603421721</c:v>
-                </c:pt>
-                <c:pt idx="183">
-                  <c:v>269.73837725430519</c:v>
-                </c:pt>
-                <c:pt idx="184">
-                  <c:v>291.73088543957084</c:v>
-                </c:pt>
-                <c:pt idx="185">
-                  <c:v>313.34314605247749</c:v>
-                </c:pt>
-                <c:pt idx="186">
-                  <c:v>334.51136082030922</c:v>
-                </c:pt>
-                <c:pt idx="187">
-                  <c:v>353.72618680656666</c:v>
-                </c:pt>
-                <c:pt idx="188">
-                  <c:v>11.56530834200808</c:v>
-                </c:pt>
-                <c:pt idx="189">
-                  <c:v>24.543686236721982</c:v>
-                </c:pt>
-                <c:pt idx="190">
-                  <c:v>35.361353501417106</c:v>
-                </c:pt>
-                <c:pt idx="191">
-                  <c:v>45.930044596718432</c:v>
-                </c:pt>
-                <c:pt idx="192">
-                  <c:v>58.029194807943739</c:v>
-                </c:pt>
-                <c:pt idx="193">
-                  <c:v>76.096357510279091</c:v>
-                </c:pt>
-                <c:pt idx="194">
-                  <c:v>94.882266323534921</c:v>
-                </c:pt>
-                <c:pt idx="195">
-                  <c:v>110.20186754656228</c:v>
-                </c:pt>
-                <c:pt idx="196">
-                  <c:v>122.37274603117625</c:v>
-                </c:pt>
-                <c:pt idx="197">
-                  <c:v>130.39122447021987</c:v>
-                </c:pt>
-                <c:pt idx="198">
-                  <c:v>137.1871175979696</c:v>
-                </c:pt>
-                <c:pt idx="199">
-                  <c:v>144.35703439225196</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-5CC9-4475-B991-A0645E217312}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="532874584"/>
-        <c:axId val="532874912"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="532874584"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="hu-HU"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="532874912"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="532874912"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="hu-HU"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="532874584"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="hu-HU"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="hu-HU"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="hu-HU"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="smoothMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Munka1!$P$4:$P$203</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="200"/>
-                <c:pt idx="0">
-                  <c:v>302.49889336399315</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>302.51381130261962</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>302.53176129316813</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>302.54742354499808</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>302.56022144390323</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>302.57041964757622</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>302.58049931630921</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>302.59658355571634</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>302.61515381155743</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>302.63609455105092</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>302.65755047075243</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>302.67809625260304</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>302.34456362910174</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>302.35944827940153</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>302.72400266425961</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>302.73340798082069</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>302.74474170093384</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>302.75905141665885</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>302.77575762450738</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>302.79434031238196</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>302.80846442558072</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>302.81816569015319</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>302.82538984823304</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>302.83210401259419</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>302.83968608055557</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>302.85039311770839</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>302.86621435356477</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>302.88304697296428</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>302.89897184972546</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>302.91179815758824</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>302.92111678096876</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>302.93278573131096</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>302.94805213798975</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>302.96567100976756</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>302.98779799941491</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>303.00885819478651</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>303.02980513771678</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>302.69593470516952</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>302.71177706239968</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>303.07545142264001</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>303.08499823232063</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>303.09630420093384</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>303.10984877602124</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>303.12755003156951</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>303.14557136738864</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>303.15923852948822</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>303.16952782513943</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>303.17678033454115</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>303.18342894131354</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>303.19088912277505</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>303.20192882992922</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>303.21774430068149</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>303.23474231605354</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>303.25148570491655</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>303.26305955957662</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>303.2730745213201</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>303.28443061598722</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>303.29798559470805</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>303.31752408044002</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>303.33860386035911</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>303.3602306962967</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>303.38043462029015</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>303.04828446234177</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>303.06372408487704</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>303.42664074710103</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>303.43678832483766</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>303.44729253325693</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>303.46116422701778</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>303.47966499927361</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>303.49568525861673</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>303.51091759659425</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>303.52099468884353</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>303.52812463549242</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>303.53475597743181</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>303.54244562673028</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>303.55342331299875</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>303.56865593022997</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>303.58668333216804</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>303.60172688597828</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>303.61457289964221</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>303.62492398475069</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>303.6353313061436</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>303.65020349118021</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>303.66850389978498</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>303.68913930838528</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>303.71085365154153</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>303.73163761471949</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>303.39897036874356</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>303.4141242924992</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>303.77833277141985</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>303.78743716625326</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>303.79868525000364</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>303.81349439540725</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>303.82942726101714</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>303.84804298778272</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>303.86215595974107</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>303.87213369365872</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>303.8795153364905</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>303.88601471838103</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>303.89357069731722</c:v>
-                </c:pt>
-                <c:pt idx="100">
-                  <c:v>303.90430476042252</c:v>
-                </c:pt>
-                <c:pt idx="101">
-                  <c:v>303.91975443543549</c:v>
-                </c:pt>
-                <c:pt idx="102">
-                  <c:v>303.93643496346726</c:v>
-                </c:pt>
-                <c:pt idx="103">
-                  <c:v>303.95280624364227</c:v>
-                </c:pt>
-                <c:pt idx="104">
-                  <c:v>303.96576274918101</c:v>
-                </c:pt>
-                <c:pt idx="105">
-                  <c:v>303.97584542982202</c:v>
-                </c:pt>
-                <c:pt idx="106">
-                  <c:v>303.98689669819089</c:v>
-                </c:pt>
-                <c:pt idx="107">
-                  <c:v>304.00113652116994</c:v>
-                </c:pt>
-                <c:pt idx="108">
-                  <c:v>304.0184826183289</c:v>
-                </c:pt>
-                <c:pt idx="109">
-                  <c:v>304.04038073806646</c:v>
-                </c:pt>
-                <c:pt idx="110">
-                  <c:v>304.06136679329876</c:v>
-                </c:pt>
-                <c:pt idx="111">
-                  <c:v>304.08156681409656</c:v>
-                </c:pt>
-                <c:pt idx="112">
-                  <c:v>304.10007652537519</c:v>
-                </c:pt>
-                <c:pt idx="113">
-                  <c:v>303.76477301235644</c:v>
-                </c:pt>
-                <c:pt idx="114">
-                  <c:v>304.12789361694593</c:v>
-                </c:pt>
-                <c:pt idx="115">
-                  <c:v>304.13865129706392</c:v>
-                </c:pt>
-                <c:pt idx="116">
-                  <c:v>304.1501031425754</c:v>
-                </c:pt>
-                <c:pt idx="117">
-                  <c:v>304.16315722256621</c:v>
-                </c:pt>
-                <c:pt idx="118">
-                  <c:v>304.1810190341597</c:v>
-                </c:pt>
-                <c:pt idx="119">
-                  <c:v>304.19838860736627</c:v>
-                </c:pt>
-                <c:pt idx="120">
-                  <c:v>304.21296606916451</c:v>
-                </c:pt>
-                <c:pt idx="121">
-                  <c:v>304.22340351292632</c:v>
-                </c:pt>
-                <c:pt idx="122">
-                  <c:v>304.23037535782186</c:v>
-                </c:pt>
-                <c:pt idx="123">
-                  <c:v>304.23708168731355</c:v>
-                </c:pt>
-                <c:pt idx="124">
-                  <c:v>304.24429566076719</c:v>
-                </c:pt>
-                <c:pt idx="125">
-                  <c:v>304.2549754005226</c:v>
-                </c:pt>
-                <c:pt idx="126">
-                  <c:v>304.26887697662534</c:v>
-                </c:pt>
-                <c:pt idx="127">
-                  <c:v>304.28706198196602</c:v>
-                </c:pt>
-                <c:pt idx="128">
-                  <c:v>304.30347084518792</c:v>
-                </c:pt>
-                <c:pt idx="129">
-                  <c:v>304.3158173233507</c:v>
-                </c:pt>
-                <c:pt idx="130">
-                  <c:v>304.32683029923305</c:v>
-                </c:pt>
-                <c:pt idx="131">
-                  <c:v>304.33713873138333</c:v>
-                </c:pt>
-                <c:pt idx="132">
-                  <c:v>304.35074069398036</c:v>
-                </c:pt>
-                <c:pt idx="133">
-                  <c:v>304.36970710001486</c:v>
-                </c:pt>
-                <c:pt idx="134">
-                  <c:v>304.39016216781238</c:v>
-                </c:pt>
-                <c:pt idx="135">
-                  <c:v>304.41105911844897</c:v>
-                </c:pt>
-                <c:pt idx="136">
-                  <c:v>304.43152038262173</c:v>
-                </c:pt>
-                <c:pt idx="137">
-                  <c:v>304.45065167862487</c:v>
-                </c:pt>
-                <c:pt idx="138">
-                  <c:v>304.1142327327492</c:v>
-                </c:pt>
-                <c:pt idx="139">
-                  <c:v>304.4786792622408</c:v>
-                </c:pt>
-                <c:pt idx="140">
-                  <c:v>304.48980047557899</c:v>
-                </c:pt>
-                <c:pt idx="141">
-                  <c:v>304.49926103650699</c:v>
-                </c:pt>
-                <c:pt idx="142">
-                  <c:v>304.51340314438562</c:v>
-                </c:pt>
-                <c:pt idx="143">
-                  <c:v>304.53086154297733</c:v>
-                </c:pt>
-                <c:pt idx="144">
-                  <c:v>304.54770930628973</c:v>
-                </c:pt>
-                <c:pt idx="145">
-                  <c:v>304.56377493148136</c:v>
-                </c:pt>
-                <c:pt idx="146">
-                  <c:v>304.57424878922808</c:v>
-                </c:pt>
-                <c:pt idx="147">
-                  <c:v>304.58149674508417</c:v>
-                </c:pt>
-                <c:pt idx="148">
-                  <c:v>304.5881257713674</c:v>
-                </c:pt>
-                <c:pt idx="149">
-                  <c:v>304.5954306074056</c:v>
-                </c:pt>
-                <c:pt idx="150">
-                  <c:v>304.60518530366528</c:v>
-                </c:pt>
-                <c:pt idx="151">
-                  <c:v>304.61930922121087</c:v>
-                </c:pt>
-                <c:pt idx="152">
-                  <c:v>304.63737135686245</c:v>
-                </c:pt>
-                <c:pt idx="153">
-                  <c:v>304.65342067224913</c:v>
-                </c:pt>
-                <c:pt idx="154">
-                  <c:v>304.66657088299553</c:v>
-                </c:pt>
-                <c:pt idx="155">
-                  <c:v>304.67750850880009</c:v>
-                </c:pt>
-                <c:pt idx="156">
-                  <c:v>304.68702111848722</c:v>
-                </c:pt>
-                <c:pt idx="157">
-                  <c:v>304.70193966819926</c:v>
-                </c:pt>
-                <c:pt idx="158">
-                  <c:v>304.71945451963705</c:v>
-                </c:pt>
-                <c:pt idx="159">
-                  <c:v>304.73943760473946</c:v>
-                </c:pt>
-                <c:pt idx="160">
-                  <c:v>304.76096599794505</c:v>
-                </c:pt>
-                <c:pt idx="161">
-                  <c:v>304.78170438044145</c:v>
-                </c:pt>
-                <c:pt idx="162">
-                  <c:v>304.80054859882847</c:v>
-                </c:pt>
-                <c:pt idx="163">
-                  <c:v>304.46439547128023</c:v>
-                </c:pt>
-                <c:pt idx="164">
-                  <c:v>304.83034781966973</c:v>
-                </c:pt>
-                <c:pt idx="165">
-                  <c:v>304.83987954595699</c:v>
-                </c:pt>
-                <c:pt idx="166">
-                  <c:v>304.8503296718165</c:v>
-                </c:pt>
-                <c:pt idx="167">
-                  <c:v>304.86369567709005</c:v>
-                </c:pt>
-                <c:pt idx="168">
-                  <c:v>304.87976593318143</c:v>
-                </c:pt>
-                <c:pt idx="169">
-                  <c:v>304.89893834608608</c:v>
-                </c:pt>
-                <c:pt idx="170">
-                  <c:v>304.91402465006604</c:v>
-                </c:pt>
-                <c:pt idx="171">
-                  <c:v>304.92491643263946</c:v>
-                </c:pt>
-                <c:pt idx="172">
-                  <c:v>304.93257771691287</c:v>
-                </c:pt>
-                <c:pt idx="173">
-                  <c:v>304.93931596721575</c:v>
-                </c:pt>
-                <c:pt idx="174">
-                  <c:v>304.94630016982433</c:v>
-                </c:pt>
-                <c:pt idx="175">
-                  <c:v>304.95561135159733</c:v>
-                </c:pt>
-                <c:pt idx="176">
-                  <c:v>304.97003853781871</c:v>
-                </c:pt>
-                <c:pt idx="177">
-                  <c:v>304.98643922852506</c:v>
-                </c:pt>
-                <c:pt idx="178">
-                  <c:v>305.00346681343342</c:v>
-                </c:pt>
-                <c:pt idx="179">
-                  <c:v>305.01771927172223</c:v>
-                </c:pt>
-                <c:pt idx="180">
-                  <c:v>305.02746191191278</c:v>
-                </c:pt>
-                <c:pt idx="181">
-                  <c:v>305.0384311941412</c:v>
-                </c:pt>
-                <c:pt idx="182">
-                  <c:v>305.0515586526779</c:v>
-                </c:pt>
-                <c:pt idx="183">
-                  <c:v>305.06810388403744</c:v>
-                </c:pt>
-                <c:pt idx="184">
-                  <c:v>305.08958094281206</c:v>
-                </c:pt>
-                <c:pt idx="185">
-                  <c:v>305.1106866660669</c:v>
-                </c:pt>
-                <c:pt idx="186">
-                  <c:v>305.1313587508011</c:v>
-                </c:pt>
-                <c:pt idx="187">
-                  <c:v>305.15012322930329</c:v>
-                </c:pt>
-                <c:pt idx="188">
-                  <c:v>304.81598174642772</c:v>
-                </c:pt>
-                <c:pt idx="189">
-                  <c:v>305.18021844359055</c:v>
-                </c:pt>
-                <c:pt idx="190">
-                  <c:v>305.19078257177875</c:v>
-                </c:pt>
-                <c:pt idx="191">
-                  <c:v>305.20110355917649</c:v>
-                </c:pt>
-                <c:pt idx="192">
-                  <c:v>305.21291913555467</c:v>
-                </c:pt>
-                <c:pt idx="193">
-                  <c:v>305.2305628491311</c:v>
-                </c:pt>
-                <c:pt idx="194">
-                  <c:v>305.24890846320659</c:v>
-                </c:pt>
-                <c:pt idx="195">
-                  <c:v>305.26386901127591</c:v>
-                </c:pt>
-                <c:pt idx="196">
-                  <c:v>305.2757546347961</c:v>
-                </c:pt>
-                <c:pt idx="197">
-                  <c:v>305.2835851801467</c:v>
-                </c:pt>
-                <c:pt idx="198">
-                  <c:v>305.29022179452926</c:v>
-                </c:pt>
-                <c:pt idx="199">
-                  <c:v>305.29722366639868</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-66BB-40AA-A216-93664DFD85D2}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Munka1!$F$4:$F$203</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="200"/>
-                <c:pt idx="0">
-                  <c:v>302.43160999999998</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>302.43160999999998</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>302.43160999999998</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>302.43160999999998</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>302.51950099999999</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>302.51950099999999</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>302.51950099999999</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>302.51950099999999</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>302.51950099999999</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>302.51950099999999</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>302.60739100000001</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>302.60739100000001</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>302.60739100000001</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>302.60739100000001</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>302.69528200000002</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>302.69528200000002</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>302.69528200000002</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>302.69528200000002</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>302.69528200000002</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>302.69528200000002</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>302.78317299999998</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>302.78317299999998</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>302.78317299999998</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>302.78317299999998</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>302.78317299999998</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>302.78317299999998</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>302.78317299999998</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>302.78317299999998</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>302.78317299999998</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>302.87106299999999</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>302.87106299999999</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>302.87106299999999</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>302.87106299999999</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>302.87106299999999</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>302.87106299999999</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>302.95895400000001</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>302.95895400000001</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>302.95895400000001</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>302.95895400000001</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>303.04684400000002</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>303.04684400000002</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>303.04684400000002</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>303.04684400000002</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>303.04684400000002</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>303.04684400000002</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>303.04684400000002</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>303.13473499999998</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>303.13473499999998</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>303.13473499999998</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>303.13473499999998</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>303.13473499999998</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>303.13473499999998</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>303.13473499999998</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>303.13473499999998</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>303.22262599999999</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>303.22262599999999</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>303.22262599999999</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>303.22262599999999</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>303.22262599999999</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>303.22262599999999</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>303.31051600000001</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>303.31051600000001</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>303.31051600000001</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>303.31051600000001</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>303.39840700000002</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>303.39840700000002</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>303.39840700000002</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>303.39840700000002</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>303.39840700000002</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>303.39840700000002</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>303.48629799999998</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>303.48629799999998</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>303.48629799999998</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>303.48629799999998</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>303.48629799999998</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>303.48629799999998</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>303.48629799999998</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>303.48629799999998</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>303.48629799999998</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>303.57418799999999</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>303.57418799999999</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>303.57418799999999</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>303.57418799999999</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>303.57418799999999</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>303.57418799999999</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>303.66207900000001</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>303.66207900000001</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>303.66207900000001</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>303.66207900000001</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>303.74996900000002</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>303.74996900000002</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>303.74996900000002</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>303.74996900000002</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>303.74996900000002</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>303.74996900000002</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>303.74996900000002</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>303.83785999999998</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>303.83785999999998</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>303.83785999999998</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>303.83785999999998</c:v>
-                </c:pt>
-                <c:pt idx="100">
-                  <c:v>303.83785999999998</c:v>
-                </c:pt>
-                <c:pt idx="101">
-                  <c:v>303.83785999999998</c:v>
-                </c:pt>
-                <c:pt idx="102">
-                  <c:v>303.83785999999998</c:v>
-                </c:pt>
-                <c:pt idx="103">
-                  <c:v>303.83785999999998</c:v>
-                </c:pt>
-                <c:pt idx="104">
-                  <c:v>303.92575099999999</c:v>
-                </c:pt>
-                <c:pt idx="105">
-                  <c:v>303.92575099999999</c:v>
-                </c:pt>
-                <c:pt idx="106">
-                  <c:v>303.92575099999999</c:v>
-                </c:pt>
-                <c:pt idx="107">
-                  <c:v>303.92575099999999</c:v>
-                </c:pt>
-                <c:pt idx="108">
-                  <c:v>303.92575099999999</c:v>
-                </c:pt>
-                <c:pt idx="109">
-                  <c:v>303.92575099999999</c:v>
-                </c:pt>
-                <c:pt idx="110">
-                  <c:v>304.01364100000001</c:v>
-                </c:pt>
-                <c:pt idx="111">
-                  <c:v>304.01364100000001</c:v>
-                </c:pt>
-                <c:pt idx="112">
-                  <c:v>304.01364100000001</c:v>
-                </c:pt>
-                <c:pt idx="113">
-                  <c:v>304.01364100000001</c:v>
-                </c:pt>
-                <c:pt idx="114">
-                  <c:v>304.10153200000002</c:v>
-                </c:pt>
-                <c:pt idx="115">
-                  <c:v>304.10153200000002</c:v>
-                </c:pt>
-                <c:pt idx="116">
-                  <c:v>304.10153200000002</c:v>
-                </c:pt>
-                <c:pt idx="117">
-                  <c:v>304.10153200000002</c:v>
-                </c:pt>
-                <c:pt idx="118">
-                  <c:v>304.10153200000002</c:v>
-                </c:pt>
-                <c:pt idx="119">
-                  <c:v>304.10153200000002</c:v>
-                </c:pt>
-                <c:pt idx="120">
-                  <c:v>304.10153200000002</c:v>
-                </c:pt>
-                <c:pt idx="121">
-                  <c:v>304.18942299999998</c:v>
-                </c:pt>
-                <c:pt idx="122">
-                  <c:v>304.18942299999998</c:v>
-                </c:pt>
-                <c:pt idx="123">
-                  <c:v>304.18942299999998</c:v>
-                </c:pt>
-                <c:pt idx="124">
-                  <c:v>304.18942299999998</c:v>
-                </c:pt>
-                <c:pt idx="125">
-                  <c:v>304.18942299999998</c:v>
-                </c:pt>
-                <c:pt idx="126">
-                  <c:v>304.18942299999998</c:v>
-                </c:pt>
-                <c:pt idx="127">
-                  <c:v>304.18942299999998</c:v>
-                </c:pt>
-                <c:pt idx="128">
-                  <c:v>304.18942299999998</c:v>
-                </c:pt>
-                <c:pt idx="129">
-                  <c:v>304.27731299999999</c:v>
-                </c:pt>
-                <c:pt idx="130">
-                  <c:v>304.27731299999999</c:v>
-                </c:pt>
-                <c:pt idx="131">
-                  <c:v>304.27731299999999</c:v>
-                </c:pt>
-                <c:pt idx="132">
-                  <c:v>304.27731299999999</c:v>
-                </c:pt>
-                <c:pt idx="133">
-                  <c:v>304.27731299999999</c:v>
-                </c:pt>
-                <c:pt idx="134">
-                  <c:v>304.27731299999999</c:v>
-                </c:pt>
-                <c:pt idx="135">
-                  <c:v>304.27731299999999</c:v>
-                </c:pt>
-                <c:pt idx="136">
-                  <c:v>304.36520400000001</c:v>
-                </c:pt>
-                <c:pt idx="137">
-                  <c:v>304.36520400000001</c:v>
-                </c:pt>
-                <c:pt idx="138">
-                  <c:v>304.36520400000001</c:v>
-                </c:pt>
-                <c:pt idx="139">
-                  <c:v>304.45309400000002</c:v>
-                </c:pt>
-                <c:pt idx="140">
-                  <c:v>304.45309400000002</c:v>
-                </c:pt>
-                <c:pt idx="141">
-                  <c:v>304.45309400000002</c:v>
-                </c:pt>
-                <c:pt idx="142">
-                  <c:v>304.45309400000002</c:v>
-                </c:pt>
-                <c:pt idx="143">
-                  <c:v>304.45309400000002</c:v>
-                </c:pt>
-                <c:pt idx="144">
-                  <c:v>304.45309400000002</c:v>
-                </c:pt>
-                <c:pt idx="145">
-                  <c:v>304.45309400000002</c:v>
-                </c:pt>
-                <c:pt idx="146">
-                  <c:v>304.54098499999998</c:v>
-                </c:pt>
-                <c:pt idx="147">
-                  <c:v>304.54098499999998</c:v>
-                </c:pt>
-                <c:pt idx="148">
-                  <c:v>304.54098499999998</c:v>
-                </c:pt>
-                <c:pt idx="149">
-                  <c:v>304.54098499999998</c:v>
-                </c:pt>
-                <c:pt idx="150">
-                  <c:v>304.54098499999998</c:v>
-                </c:pt>
-                <c:pt idx="151">
-                  <c:v>304.54098499999998</c:v>
-                </c:pt>
-                <c:pt idx="152">
-                  <c:v>304.54098499999998</c:v>
-                </c:pt>
-                <c:pt idx="153">
-                  <c:v>304.54098499999998</c:v>
-                </c:pt>
-                <c:pt idx="154">
-                  <c:v>304.62887599999999</c:v>
-                </c:pt>
-                <c:pt idx="155">
-                  <c:v>304.62887599999999</c:v>
-                </c:pt>
-                <c:pt idx="156">
-                  <c:v>304.62887599999999</c:v>
-                </c:pt>
-                <c:pt idx="157">
-                  <c:v>304.62887599999999</c:v>
-                </c:pt>
-                <c:pt idx="158">
-                  <c:v>304.62887599999999</c:v>
-                </c:pt>
-                <c:pt idx="159">
-                  <c:v>304.62887599999999</c:v>
-                </c:pt>
-                <c:pt idx="160">
-                  <c:v>304.62887599999999</c:v>
-                </c:pt>
-                <c:pt idx="161">
-                  <c:v>304.71676600000001</c:v>
-                </c:pt>
-                <c:pt idx="162">
-                  <c:v>304.71676600000001</c:v>
-                </c:pt>
-                <c:pt idx="163">
-                  <c:v>304.71676600000001</c:v>
-                </c:pt>
-                <c:pt idx="164">
-                  <c:v>304.80465700000002</c:v>
-                </c:pt>
-                <c:pt idx="165">
-                  <c:v>304.80465700000002</c:v>
-                </c:pt>
-                <c:pt idx="166">
-                  <c:v>304.80465700000002</c:v>
-                </c:pt>
-                <c:pt idx="167">
-                  <c:v>304.80465700000002</c:v>
-                </c:pt>
-                <c:pt idx="168">
-                  <c:v>304.80465700000002</c:v>
-                </c:pt>
-                <c:pt idx="169">
-                  <c:v>304.80465700000002</c:v>
-                </c:pt>
-                <c:pt idx="170">
-                  <c:v>304.80465700000002</c:v>
-                </c:pt>
-                <c:pt idx="171">
-                  <c:v>304.89254799999998</c:v>
-                </c:pt>
-                <c:pt idx="172">
-                  <c:v>304.89254799999998</c:v>
-                </c:pt>
-                <c:pt idx="173">
-                  <c:v>304.89254799999998</c:v>
-                </c:pt>
-                <c:pt idx="174">
-                  <c:v>304.89254799999998</c:v>
-                </c:pt>
-                <c:pt idx="175">
-                  <c:v>304.89254799999998</c:v>
-                </c:pt>
-                <c:pt idx="176">
-                  <c:v>304.89254799999998</c:v>
-                </c:pt>
-                <c:pt idx="177">
-                  <c:v>304.89254799999998</c:v>
-                </c:pt>
-                <c:pt idx="178">
-                  <c:v>304.89254799999998</c:v>
-                </c:pt>
-                <c:pt idx="179">
-                  <c:v>304.89254799999998</c:v>
-                </c:pt>
-                <c:pt idx="180">
-                  <c:v>304.98043799999999</c:v>
-                </c:pt>
-                <c:pt idx="181">
-                  <c:v>304.98043799999999</c:v>
-                </c:pt>
-                <c:pt idx="182">
-                  <c:v>304.98043799999999</c:v>
-                </c:pt>
-                <c:pt idx="183">
-                  <c:v>304.98043799999999</c:v>
-                </c:pt>
-                <c:pt idx="184">
-                  <c:v>304.98043799999999</c:v>
-                </c:pt>
-                <c:pt idx="185">
-                  <c:v>304.98043799999999</c:v>
-                </c:pt>
-                <c:pt idx="186">
-                  <c:v>305.06832900000001</c:v>
-                </c:pt>
-                <c:pt idx="187">
-                  <c:v>305.06832900000001</c:v>
-                </c:pt>
-                <c:pt idx="188">
-                  <c:v>305.06832900000001</c:v>
-                </c:pt>
-                <c:pt idx="189">
-                  <c:v>305.15621900000002</c:v>
-                </c:pt>
-                <c:pt idx="190">
-                  <c:v>305.15621900000002</c:v>
-                </c:pt>
-                <c:pt idx="191">
-                  <c:v>305.15621900000002</c:v>
-                </c:pt>
-                <c:pt idx="192">
-                  <c:v>305.15621900000002</c:v>
-                </c:pt>
-                <c:pt idx="193">
-                  <c:v>305.15621900000002</c:v>
-                </c:pt>
-                <c:pt idx="194">
-                  <c:v>305.15621900000002</c:v>
-                </c:pt>
-                <c:pt idx="195">
-                  <c:v>305.15621900000002</c:v>
-                </c:pt>
-                <c:pt idx="196">
-                  <c:v>305.24410999999998</c:v>
-                </c:pt>
-                <c:pt idx="197">
-                  <c:v>305.24410999999998</c:v>
-                </c:pt>
-                <c:pt idx="198">
-                  <c:v>305.24410999999998</c:v>
-                </c:pt>
-                <c:pt idx="199">
-                  <c:v>305.24410999999998</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-66BB-40AA-A216-93664DFD85D2}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="592657120"/>
-        <c:axId val="592653840"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="592657120"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="hu-HU"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="592653840"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="592653840"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="hu-HU"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="592657120"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="hu-HU"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -5024,86 +2623,6 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -6175,1038 +3694,6 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -7280,78 +3767,6 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>285748</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>89647</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>32</xdr:col>
-      <xdr:colOff>302558</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>123264</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="10" name="Diagram 9">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D3D6705A-406B-4A51-BA85-A7E3978CF5BB}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>599513</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>134472</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>313766</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>78442</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="13" name="Diagram 12">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B4B72308-6C84-44CD-BD6C-01B2650062CC}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -7660,7 +4075,7 @@
   <dimension ref="A1:P204"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17:E18"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7690,13 +4105,13 @@
       <c r="M1" s="5"/>
     </row>
     <row r="2" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
       <c r="G2" s="2">
         <f>MIN(B4:B203)</f>
         <v>26512</v>
@@ -8496,11 +4911,11 @@
       <c r="F16" s="6">
         <v>302.60739100000001</v>
       </c>
-      <c r="G16" s="8">
+      <c r="G16" s="7">
         <f t="shared" si="0"/>
         <v>136</v>
       </c>
-      <c r="H16" s="8">
+      <c r="H16" s="7">
         <f t="shared" si="1"/>
         <v>-9352</v>
       </c>
@@ -8520,7 +4935,7 @@
         <f t="shared" si="5"/>
         <v>2.3143227782800265E-3</v>
       </c>
-      <c r="M16" s="8">
+      <c r="M16" s="7">
         <f t="shared" si="6"/>
         <v>860</v>
       </c>
@@ -8557,11 +4972,11 @@
       <c r="F17" s="6">
         <v>302.60739100000001</v>
       </c>
-      <c r="G17" s="8">
+      <c r="G17" s="7">
         <f t="shared" si="0"/>
         <v>2824</v>
       </c>
-      <c r="H17" s="8">
+      <c r="H17" s="7">
         <f t="shared" si="1"/>
         <v>-9800</v>
       </c>
@@ -8581,7 +4996,7 @@
         <f t="shared" si="5"/>
         <v>4.4652883631093432E-2</v>
       </c>
-      <c r="M17" s="8">
+      <c r="M17" s="7">
         <f t="shared" si="6"/>
         <v>860</v>
       </c>
@@ -10021,11 +6436,11 @@
       <c r="F41" s="6">
         <v>302.95895400000001</v>
       </c>
-      <c r="G41" s="8">
+      <c r="G41" s="7">
         <f t="shared" si="0"/>
         <v>104</v>
       </c>
-      <c r="H41" s="8">
+      <c r="H41" s="7">
         <f t="shared" si="1"/>
         <v>-9352</v>
       </c>
@@ -10045,7 +6460,7 @@
         <f t="shared" si="5"/>
         <v>1.7698280377842145E-3</v>
       </c>
-      <c r="M41" s="8">
+      <c r="M41" s="7">
         <f t="shared" si="6"/>
         <v>861</v>
       </c>
@@ -10082,11 +6497,11 @@
       <c r="F42" s="6">
         <v>302.95895400000001</v>
       </c>
-      <c r="G42" s="8">
+      <c r="G42" s="7">
         <f t="shared" si="0"/>
         <v>2936</v>
       </c>
-      <c r="H42" s="8">
+      <c r="H42" s="7">
         <f t="shared" si="1"/>
         <v>-9688</v>
       </c>
@@ -10106,7 +6521,7 @@
         <f t="shared" si="5"/>
         <v>4.6832533047885976E-2</v>
       </c>
-      <c r="M42" s="8">
+      <c r="M42" s="7">
         <f t="shared" si="6"/>
         <v>861</v>
       </c>

</xml_diff>